<commit_message>
print against 2018 data
- database more resilient against weird excel data.
- CTeam replaced by seed->team map.
- seeded teams for elimination rounds read (but not displayed yet).
- fixed benjy style layout... 3rd place game went missing and without bg fill.
- internationalization of match numbers in benjy layout.
- optional group stage heading for calendar.
- updated 2022 sheet to conform to new common schema.
</commit_message>
<xml_diff>
--- a/tournaments/2022-mens-world-cup.xlsx
+++ b/tournaments/2022-mens-world-cup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\tournaments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D65013-94EC-44D2-9A3B-CE173F352922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F652C7-7AF1-4956-A3E6-D7B02C51107A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2627" yWindow="2700" windowWidth="19200" windowHeight="10073" activeTab="2" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="176">
   <si>
     <t>A1</t>
   </si>
@@ -227,12 +227,6 @@
   </si>
   <si>
     <t>match</t>
-  </si>
-  <si>
-    <t>home</t>
-  </si>
-  <si>
-    <t>away</t>
   </si>
   <si>
     <t>time</t>
@@ -590,6 +584,18 @@
   </si>
   <si>
     <t>جام جهانی 2022 برنامه و کارت امتیاز</t>
+  </si>
+  <si>
+    <t>home-seed</t>
+  </si>
+  <si>
+    <t>away-seed</t>
+  </si>
+  <si>
+    <t>home-team</t>
+  </si>
+  <si>
+    <t>away-team</t>
   </si>
 </sst>
 </file>
@@ -696,14 +702,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}" name="matches" displayName="matches" ref="A1:I65" totalsRowShown="0">
-  <autoFilter ref="A1:I65" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}" name="matches" displayName="matches" ref="A1:K65" totalsRowShown="0">
+  <autoFilter ref="A1:K65" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{35D3E9F5-BB3B-4940-9EB6-C927FD84875C}" name="match"/>
-    <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home"/>
-    <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away"/>
+    <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home-seed"/>
+    <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away-seed"/>
     <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time"/>
     <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{FC876643-4BF9-4FDA-A0ED-DF50FF384B1F}" name="home-team"/>
+    <tableColumn id="10" xr3:uid="{E5D59926-7D0A-4689-A049-F55DB0E286E9}" name="away-team"/>
     <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="3"/>
     <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="1"/>
@@ -1045,350 +1053,350 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" t="s">
         <v>128</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>129</v>
       </c>
-      <c r="E10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F10" t="s">
-        <v>131</v>
-      </c>
       <c r="G10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1403,51 +1411,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="4" max="4" width="16.46875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5859375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.17578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.76171875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.3515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.9375" style="2"/>
+    <col min="8" max="8" width="12.5859375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.17578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.76171875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.3515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1463,12 +1478,12 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1484,12 +1499,12 @@
       <c r="E3">
         <v>3</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1505,12 +1520,12 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1526,12 +1541,12 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1547,12 +1562,12 @@
       <c r="E6">
         <v>8</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1568,12 +1583,12 @@
       <c r="E7">
         <v>7</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1589,12 +1604,12 @@
       <c r="E8">
         <v>6</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1610,12 +1625,12 @@
       <c r="E9">
         <v>5</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1631,12 +1646,12 @@
       <c r="E10">
         <v>4</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1652,12 +1667,12 @@
       <c r="E11">
         <v>3</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1673,12 +1688,12 @@
       <c r="E12">
         <v>2</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1694,12 +1709,12 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1715,12 +1730,12 @@
       <c r="E14">
         <v>8</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1736,12 +1751,12 @@
       <c r="E15">
         <v>7</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1757,12 +1772,12 @@
       <c r="E16">
         <v>6</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1778,12 +1793,12 @@
       <c r="E17">
         <v>5</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1799,12 +1814,12 @@
       <c r="E18">
         <v>4</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1820,12 +1835,12 @@
       <c r="E19">
         <v>3</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1841,12 +1856,12 @@
       <c r="E20">
         <v>2</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1862,12 +1877,12 @@
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1883,12 +1898,12 @@
       <c r="E22">
         <v>8</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1904,12 +1919,12 @@
       <c r="E23">
         <v>7</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1925,12 +1940,12 @@
       <c r="E24">
         <v>6</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1946,12 +1961,12 @@
       <c r="E25">
         <v>5</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1967,12 +1982,12 @@
       <c r="E26">
         <v>4</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1988,12 +2003,12 @@
       <c r="E27">
         <v>3</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2009,12 +2024,12 @@
       <c r="E28">
         <v>2</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2030,12 +2045,12 @@
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2051,12 +2066,12 @@
       <c r="E30">
         <v>8</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2072,12 +2087,12 @@
       <c r="E31">
         <v>7</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2093,12 +2108,12 @@
       <c r="E32">
         <v>6</v>
       </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2114,12 +2129,12 @@
       <c r="E33">
         <v>5</v>
       </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2135,12 +2150,12 @@
       <c r="E34">
         <v>4</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2156,12 +2171,12 @@
       <c r="E35">
         <v>3</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2177,12 +2192,12 @@
       <c r="E36">
         <v>2</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2198,12 +2213,12 @@
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2219,12 +2234,12 @@
       <c r="E38">
         <v>8</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2240,12 +2255,12 @@
       <c r="E39">
         <v>7</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2261,12 +2276,12 @@
       <c r="E40">
         <v>6</v>
       </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2282,12 +2297,12 @@
       <c r="E41">
         <v>5</v>
       </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2303,12 +2318,12 @@
       <c r="E42">
         <v>4</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2324,12 +2339,12 @@
       <c r="E43">
         <v>3</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2345,12 +2360,12 @@
       <c r="E44">
         <v>2</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2366,12 +2381,12 @@
       <c r="E45">
         <v>1</v>
       </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2387,12 +2402,12 @@
       <c r="E46">
         <v>8</v>
       </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2408,12 +2423,12 @@
       <c r="E47">
         <v>7</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2429,12 +2444,12 @@
       <c r="E48">
         <v>6</v>
       </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2450,12 +2465,12 @@
       <c r="E49">
         <v>5</v>
       </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2471,12 +2486,12 @@
       <c r="E50">
         <v>2</v>
       </c>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2492,12 +2507,12 @@
       <c r="E51">
         <v>4</v>
       </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2513,12 +2528,12 @@
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2534,12 +2549,12 @@
       <c r="E53">
         <v>3</v>
       </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2555,12 +2570,12 @@
       <c r="E54">
         <v>8</v>
       </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2576,12 +2591,12 @@
       <c r="E55">
         <v>6</v>
       </c>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2597,12 +2612,12 @@
       <c r="E56">
         <v>7</v>
       </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2618,12 +2633,12 @@
       <c r="E57">
         <v>5</v>
       </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2639,12 +2654,12 @@
       <c r="E58">
         <v>5</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2660,12 +2675,12 @@
       <c r="E59">
         <v>7</v>
       </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2681,12 +2696,12 @@
       <c r="E60">
         <v>1</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2702,12 +2717,12 @@
       <c r="E61">
         <v>3</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2723,12 +2738,12 @@
       <c r="E62">
         <v>5</v>
       </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2744,20 +2759,20 @@
       <c r="E63">
         <v>1</v>
       </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D64" s="1">
         <v>44912.625</v>
@@ -2765,12 +2780,12 @@
       <c r="E64">
         <v>2</v>
       </c>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2786,10 +2801,10 @@
       <c r="E65">
         <v>5</v>
       </c>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2804,7 +2819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7827E4A0-E10B-4512-807E-A38B484A1AB9}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2815,10 +2830,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
@@ -2826,7 +2841,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
@@ -2834,7 +2849,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.5">
@@ -2842,7 +2857,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
@@ -2850,7 +2865,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.5">
@@ -2858,7 +2873,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.5">
@@ -2866,7 +2881,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.5">
@@ -2874,7 +2889,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.5">
@@ -2882,7 +2897,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.5">
@@ -2890,7 +2905,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.5">
@@ -2898,7 +2913,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.5">
@@ -2906,7 +2921,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.5">
@@ -2914,7 +2929,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.5">
@@ -2922,7 +2937,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.5">
@@ -2930,7 +2945,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.5">
@@ -2938,7 +2953,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.5">
@@ -2946,7 +2961,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.5">
@@ -2954,7 +2969,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.5">
@@ -2962,7 +2977,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.5">
@@ -2970,7 +2985,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.5">
@@ -2978,7 +2993,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.5">
@@ -2986,7 +3001,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.5">
@@ -2994,7 +3009,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.5">
@@ -3002,7 +3017,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.5">
@@ -3010,7 +3025,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.5">
@@ -3018,7 +3033,7 @@
         <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.5">
@@ -3026,7 +3041,7 @@
         <v>31</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.5">
@@ -3034,7 +3049,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.5">
@@ -3042,7 +3057,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.5">
@@ -3050,7 +3065,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.5">
@@ -3058,7 +3073,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.5">
@@ -3066,7 +3081,7 @@
         <v>26</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.5">
@@ -3074,7 +3089,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>